<commit_message>
Add test for ExtLookup and ExtData
Add more test for ExtLookup and ExtData for 1, 2 and 3 dimensions
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -14,11 +14,11 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="data_1d" vbProcedure="false">Horizontal!$C$5:$J$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_2d" vbProcedure="false">Horizontal!$C$5:$J$7</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="data_3d" vbProcedure="false">Horizontal!$C$5:$J$10</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="data_2db" vbProcedure="false">Horizontal!$C$8:$J$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="time" vbProcedure="false">Horizontal!$C$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="data_1d" vbProcedure="false">Vertical!$C$5:$C$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="data_2d" vbProcedure="false">Vertical!$C$5:$E$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="data_3d" vbProcedure="false">Vertical!$C$5:$H$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="data_2db" vbProcedure="false">Vertical!$F$5:$H$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="time" vbProcedure="false">Vertical!$B$5:$B$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -153,10 +153,10 @@
   <dimension ref="A4:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="F5:H12 C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
@@ -391,10 +391,10 @@
   <dimension ref="B3:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">

</xml_diff>

<commit_message>
Add test for 0d and 1d ExtConstant
Add test for ExtConstant for 0d and 1d data.
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Vertical" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" name="constant" vbProcedure="false">Horizontal!$F$7</definedName>
+    <definedName function="false" hidden="false" name="constant2" vbProcedure="false">Horizontal!$C$6</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_1d" vbProcedure="false">Horizontal!$C$5:$J$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_2d" vbProcedure="false">Horizontal!$C$5:$J$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_2db" vbProcedure="false">Horizontal!$C$8:$J$10</definedName>
@@ -152,11 +154,11 @@
   </sheetPr>
   <dimension ref="A4:J10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="F5:H12 C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
@@ -390,11 +392,11 @@
   </sheetPr>
   <dimension ref="B3:H23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="s">

</xml_diff>

<commit_message>
Corrections on some warnings/errors in external
Corrections on some warnings/errors in external and most test added to increase the coverage in this package to the maximum
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,23 +5,35 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Vertical" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Horizontal missing" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Vertical missing" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="No monotonous" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="constant" vbProcedure="false">Horizontal!$F$7</definedName>
     <definedName function="false" hidden="false" name="constant2" vbProcedure="false">Horizontal!$C$5</definedName>
+    <definedName function="false" hidden="false" name="data_1d" vbProcedure="false">'No monotonous'!$C$5:$J$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="data_1" vbProcedure="false">Horizontal!$B$17</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_1d" vbProcedure="false">Horizontal!$C$5:$J$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_2d" vbProcedure="false">Horizontal!$C$5:$J$7</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_2db" vbProcedure="false">Horizontal!$C$8:$J$10</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="time" vbProcedure="false">Horizontal!$C$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="time_1" vbProcedure="false">Horizontal!$B$16</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="data_1d" vbProcedure="false">Vertical!$C$5:$C$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="data_2d" vbProcedure="false">Vertical!$C$5:$E$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="data_2db" vbProcedure="false">Vertical!$F$5:$H$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="time" vbProcedure="false">Vertical!$B$5:$B$12</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="data_1d" vbProcedure="false">'Horizontal missing'!$C$5:$K$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="len_0" vbProcedure="false">'Horizontal missing'!$C$3:$K$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="time_missing" vbProcedure="false">'Horizontal missing'!$C$4:$K$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="data_2d_short" vbProcedure="false">'Vertical missing'!$C$5:$E$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="time_short" vbProcedure="false">'Vertical missing'!$B$5:$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="time" vbProcedure="false">'No monotonous'!$C$4:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -33,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="5">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -154,11 +166,11 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -530,7 +542,9 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -546,7 +560,9 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -742,11 +758,11 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1337,4 +1353,733 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="C9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:A7"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add warnings for missing values and extrapolation
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
   <definedNames>
     <definedName function="false" hidden="false" name="constant" vbProcedure="false">Horizontal!$F$7</definedName>
     <definedName function="false" hidden="false" name="constant2" vbProcedure="false">Horizontal!$C$5</definedName>
+    <definedName function="false" hidden="false" name="data_1" vbProcedure="false">'Horizontal missing'!$C$15:$K$15</definedName>
     <definedName function="false" hidden="false" name="data_1d" vbProcedure="false">'No monotonous'!$C$5:$J$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_1" vbProcedure="false">Horizontal!$B$17</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="data_1d" vbProcedure="false">Horizontal!$C$5:$J$5</definedName>
@@ -29,7 +30,10 @@
     <definedName function="false" hidden="false" localSheetId="1" name="data_2db" vbProcedure="false">Vertical!$F$5:$H$12</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="time" vbProcedure="false">Vertical!$B$5:$B$12</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="data_1d" vbProcedure="false">'Horizontal missing'!$C$5:$K$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="data_2d" vbProcedure="false">'Horizontal missing'!$C$16:$J$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="data_2db" vbProcedure="false">'Horizontal missing'!$C$19:$J$21</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="len_0" vbProcedure="false">'Horizontal missing'!$C$3:$K$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="time" vbProcedure="false">'Horizontal missing'!$C$15:$J$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="time_missing" vbProcedure="false">'Horizontal missing'!$C$4:$K$4</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="data_2d_short" vbProcedure="false">'Vertical missing'!$C$5:$E$6</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="time_short" vbProcedure="false">'Vertical missing'!$B$5:$B$8</definedName>
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="5">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -166,11 +170,11 @@
   </sheetPr>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -762,7 +766,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1360,13 +1364,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1628,10 +1632,211 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A19:A21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1654,7 +1859,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1950,7 +2155,7 @@
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>

</xml_diff>

<commit_message>
Solve bugs when reading data with openpyxl
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Horizontal missing" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Vertical missing" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="No monotonous" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="CaSe and Non V" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="constant" vbProcedure="false">Horizontal!$F$7</definedName>
@@ -38,6 +39,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="data_2d_short" vbProcedure="false">'Vertical missing'!$C$5:$E$6</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="time_short" vbProcedure="false">'Vertical missing'!$B$5:$B$8</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="time" vbProcedure="false">'No monotonous'!$C$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="no_constant" vbProcedure="false">'CaSe and Non V'!$B$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="series" vbProcedure="false">'CaSe and Non V'!$A$4:$F$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="unit" vbProcedure="false">'CaSe and Non V'!$A$5:$F$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -49,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="7">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -64,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9constant</t>
   </si>
 </sst>
 </file>
@@ -174,7 +184,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -766,7 +776,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1366,11 +1376,11 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1859,7 +1869,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2155,7 +2165,7 @@
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2287,4 +2297,73 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A4:F8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Making the order of Externals series more flexible
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="7">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -184,7 +184,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -757,7 +757,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -776,7 +776,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1361,7 +1361,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1380,7 +1380,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1850,7 +1850,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1869,7 +1869,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2146,7 +2146,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2159,13 +2159,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2285,13 +2285,108 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2306,11 +2401,11 @@
   </sheetPr>
   <dimension ref="A4:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -2360,7 +2455,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Split Vensim views into submodules (#283)
* untested implementation of views separator

* tests implementation and adds doc

* fixed documentation

* fixed documentation

* Small corrections

* Remove duplicated vars

* Remove subscripts dicts when possible from external objects

* remove increasing constraint in monotonic external data

* Making the order of Externals series more flexible

* addapting sketch grammar for Vensin 8.2.1

Co-authored-by: Eneko Martin Martinez <eneko.martin.martinez@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="7">
   <si>
     <t xml:space="preserve">X</t>
   </si>
@@ -184,7 +184,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -757,7 +757,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -776,7 +776,7 @@
       <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1361,7 +1361,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1380,7 +1380,7 @@
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1850,7 +1850,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1869,7 +1869,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2146,7 +2146,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2159,13 +2159,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2285,13 +2285,108 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2306,11 +2401,11 @@
   </sheetPr>
   <dimension ref="A4:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -2360,7 +2455,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Keep missing values when interpolation is not possible in external objects
</commit_message>
<xml_diff>
--- a/tests/data/input.xlsx
+++ b/tests/data/input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Horizontal" sheetId="1" state="visible" r:id="rId2"/>
@@ -181,10 +181,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -773,10 +773,10 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1376,11 +1376,11 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -1869,7 +1869,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2161,11 +2161,11 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -2405,7 +2405,7 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">

</xml_diff>